<commit_message>
aggiunto esercizio su prob programming proportion
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/BDA-syllabus.xlsx
+++ b/syllabus-and-improv/BDA-syllabus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D16686-D656-B641-9E30-BEC8AC63EECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DB9122-6E49-E843-B30D-AFF40A0866EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{A3CB9B10-4073-244F-8BBF-C57FD281AC5C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="16020" xr2:uid="{A3CB9B10-4073-244F-8BBF-C57FD281AC5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Settimana</t>
   </si>
@@ -50,12 +50,6 @@
     <t>Bayesian t-test</t>
   </si>
   <si>
-    <t>3 + 1 ogni settimana?</t>
-  </si>
-  <si>
-    <t>6 + 2 ogni due settimane?</t>
-  </si>
-  <si>
     <t>probabilita e Bayes rule</t>
   </si>
   <si>
@@ -68,33 +62,6 @@
     <t>presentazione (o elaborazione) progetti</t>
   </si>
   <si>
-    <t>Assignment vehtari</t>
-  </si>
-  <si>
-    <t>molto carino, modelli gerarchici.</t>
-  </si>
-  <si>
-    <t>potenziale assignment</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>ok come esercizi</t>
-  </si>
-  <si>
-    <t>metropolis for bioassay</t>
-  </si>
-  <si>
-    <t>assignment (da tradurre in pymc3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inference for the difference between proportions </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ok come esercizio o anche assignment. Interessante: Frank Harrell’s recommendations on how to state results in Bayesian two group comparison. </t>
-  </si>
-  <si>
     <t>bioassay con metropolis; alcuni punti avanzati facoltativi; coprire nelle esercitazioni I pre-requisiti</t>
   </si>
   <si>
@@ -147,13 +114,55 @@
   </si>
   <si>
     <t>revisione progetti?</t>
+  </si>
+  <si>
+    <t>Previsione</t>
+  </si>
+  <si>
+    <t>Sequenza effettiva</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>think bayesian, bayes rule (esempio fake news incluso + exe 2.5 arboretum)</t>
+  </si>
+  <si>
+    <t>ripresa beta; binomial likelihood; up to slide 54 (sensitivity to the prior)</t>
+  </si>
+  <si>
+    <t>finire beta-bin; 3.9, 3.10, normal-normal</t>
+  </si>
+  <si>
+    <t>reporting analysis; normal normal (esercizio likelihood)</t>
+  </si>
+  <si>
+    <t>normal normal: 5.9, 5.10 (risolti insieme) prior su varianza; MCMC island</t>
+  </si>
+  <si>
+    <t>ripresa MCMC (esercizi di implementazione: 1) island hopping; 2) bi-dimensional gridding of the normal-normal model)</t>
+  </si>
+  <si>
+    <t>settimana</t>
+  </si>
+  <si>
+    <t>contenuto</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>ripresa bayes rule (marginal, joint; fatto risolvere esempio infected | positive;  goat); finito in anticipo 20 mins</t>
+  </si>
+  <si>
+    <t>beta-binomial (beta; binomial  quickly introduced)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -177,15 +186,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <strike/>
       <sz val="12"/>
       <color rgb="FF006100"/>
@@ -202,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +220,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -234,22 +240,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{9191B0B7-01C7-CC4F-9593-AE8A1D952906}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -259,6 +291,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8DCCDB50-8E6E-E145-8C6F-1C2B0DC16C59}" name="Table1" displayName="Table1" ref="A22:D49" totalsRowShown="0">
+  <autoFilter ref="A22:D49" xr:uid="{8DCCDB50-8E6E-E145-8C6F-1C2B0DC16C59}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{49C91133-6B7D-6E4C-824B-74D0FC7ED537}" name="settimana"/>
+    <tableColumn id="2" xr3:uid="{5BA8994D-CCDC-AB44-B478-9B1CD1AB67DC}" name="data" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{F4624562-3B7D-EE4D-BFC1-AF46FFBB3BBB}" name="contenuto" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{3C90563A-2B95-9941-8373-5C9A348919D8}" name="Column1" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -558,279 +603,548 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D01C0E-36DF-B748-B91C-92F7CA25FEEF}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="184" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="43.6640625" customWidth="1"/>
-    <col min="3" max="3" width="71.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="76.6640625" customWidth="1"/>
+    <col min="4" max="4" width="57.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>0</v>
+      <c r="A4">
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="3" t="s">
-        <v>20</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="5"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="6"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>10</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>36</v>
       </c>
-      <c r="C18" t="s">
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>15</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" s="7">
+        <v>44823</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" s="7">
+        <f>B23+3</f>
+        <v>44826</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" s="7">
+        <f>B23+7</f>
+        <v>44830</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" s="8">
+        <f>B25+3</f>
+        <v>44833</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
-      <c r="B27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B27" s="7">
+        <f>B25+7</f>
+        <v>44837</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" s="7">
+        <f>B27+3</f>
+        <v>44840</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
         <v>4</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" s="7">
+        <f>B27+7</f>
+        <v>44844</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" s="8">
+        <f>B29+3</f>
+        <v>44847</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31" s="7">
+        <f>B29+7</f>
+        <v>44851</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="9"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32" s="7">
+        <f>B31+3</f>
+        <v>44854</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="9"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33" s="7">
+        <f>B31+7</f>
+        <v>44858</v>
+      </c>
+      <c r="C33" s="11"/>
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="B34" s="8">
+        <f>B33+3</f>
+        <v>44861</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>7</v>
+      </c>
+      <c r="B35" s="7">
+        <f>B33+7</f>
+        <v>44865</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" s="9"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>7</v>
+      </c>
+      <c r="B36" s="7">
+        <f>B35+3</f>
+        <v>44868</v>
+      </c>
+      <c r="C36" s="11"/>
+      <c r="D36" s="9"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>8</v>
+      </c>
+      <c r="B37" s="7">
+        <f>B35+7</f>
+        <v>44872</v>
+      </c>
+      <c r="C37" s="11"/>
+      <c r="D37" s="9"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>8</v>
+      </c>
+      <c r="B38" s="8">
+        <f>B37+3</f>
+        <v>44875</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="9"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>9</v>
+      </c>
+      <c r="B39" s="7">
+        <f>B37+7</f>
+        <v>44879</v>
+      </c>
+      <c r="C39" s="11"/>
+      <c r="D39" s="9"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>9</v>
+      </c>
+      <c r="B40" s="7">
+        <f>B39+3</f>
+        <v>44882</v>
+      </c>
+      <c r="C40" s="11"/>
+      <c r="D40" s="9"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>10</v>
+      </c>
+      <c r="B41" s="7">
+        <f>B39+7</f>
+        <v>44886</v>
+      </c>
+      <c r="C41" s="11"/>
+      <c r="D41" s="9"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>10</v>
+      </c>
+      <c r="B42" s="8">
+        <f>B41+3</f>
+        <v>44889</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="9"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>11</v>
+      </c>
+      <c r="B43" s="7">
+        <f>B41+7</f>
+        <v>44893</v>
+      </c>
+      <c r="C43" s="11"/>
+      <c r="D43" s="9"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>11</v>
+      </c>
+      <c r="B44" s="7">
+        <f>B43+3</f>
+        <v>44896</v>
+      </c>
+      <c r="C44" s="11"/>
+      <c r="D44" s="9"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>12</v>
+      </c>
+      <c r="B45" s="7">
+        <f>B43+7</f>
+        <v>44900</v>
+      </c>
+      <c r="C45" s="11"/>
+      <c r="D45" s="9"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>12</v>
+      </c>
+      <c r="B46" s="8">
+        <f>B45+3</f>
+        <v>44903</v>
+      </c>
+      <c r="C46" s="12"/>
+      <c r="D46" s="9"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>13</v>
+      </c>
+      <c r="B47" s="7">
+        <f>B45+7</f>
+        <v>44907</v>
+      </c>
+      <c r="C47" s="11"/>
+      <c r="D47" s="9"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>13</v>
+      </c>
+      <c r="B48" s="7">
+        <f>B47+3</f>
+        <v>44910</v>
+      </c>
+      <c r="C48" s="11"/>
+      <c r="D48" s="9"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>5</v>
-      </c>
-      <c r="B29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>7</v>
-      </c>
-      <c r="B31" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>8</v>
-      </c>
-      <c r="B32" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>9</v>
-      </c>
-      <c r="B33" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" t="s">
-        <v>13</v>
-      </c>
+      <c r="B49" s="7">
+        <f>B47+7</f>
+        <v>44914</v>
+      </c>
+      <c r="C49" s="11"/>
+      <c r="D49" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update prog-programming proportion with final exercise
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/BDA-syllabus.xlsx
+++ b/syllabus-and-improv/BDA-syllabus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B801BCEB-FD41-D549-982A-4B0F52884D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C4CF66-6B3A-874A-8FF1-F61300E2862C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="16020" xr2:uid="{A3CB9B10-4073-244F-8BBF-C57FD281AC5C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{A3CB9B10-4073-244F-8BBF-C57FD281AC5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -158,13 +158,13 @@
     <t>beta-binomial (beta; binomial  quickly introduced)</t>
   </si>
   <si>
-    <t>prob programming - proporzione</t>
-  </si>
-  <si>
-    <t>prob programming - proporzione + introduzione progetto e assignment</t>
-  </si>
-  <si>
     <t>exe MF: metropolis</t>
+  </si>
+  <si>
+    <t>prob programming - proporzione (fare loro implementare uniform (0,1) and uniform (0,0.2)</t>
+  </si>
+  <si>
+    <t>ripresa gridding 2d; prob programming proporzione; introduzione progetto e assignment</t>
   </si>
 </sst>
 </file>
@@ -249,7 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
@@ -272,7 +272,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -617,7 +616,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" zoomScale="184" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -974,7 +973,7 @@
         <v>44858</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D33" s="9"/>
     </row>
@@ -982,12 +981,12 @@
       <c r="A34">
         <v>6</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34" s="7">
         <f>B33+3</f>
         <v>44861</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D34" s="9"/>
     </row>
@@ -1000,7 +999,7 @@
         <v>44865</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D35" s="9"/>
     </row>

</xml_diff>

<commit_message>
updated your turn slides in (normal normal)
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/BDA-syllabus.xlsx
+++ b/syllabus-and-improv/BDA-syllabus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBBF549-05C6-3E4B-BE79-7263365783F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09BDDD0-60F3-7B46-8599-FF9E3FD459D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{A3CB9B10-4073-244F-8BBF-C57FD281AC5C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="16020" xr2:uid="{A3CB9B10-4073-244F-8BBF-C57FD281AC5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Settimana</t>
   </si>
@@ -161,16 +164,16 @@
     <t>exe MF: metropolis</t>
   </si>
   <si>
-    <t>prob programming - proporzione (fare loro implementare uniform (0,1) and uniform (0,0.2)</t>
-  </si>
-  <si>
-    <t>ripresa gridding 2d; prob programming proporzione; introduzione progetto e assignment</t>
-  </si>
-  <si>
-    <t>normal normal in pymc3</t>
-  </si>
-  <si>
-    <t>progetto e data consegna</t>
+    <t>ripresa bi-dimensional gridding; rope e esercizio classifier; presentazione assignment da Marco</t>
+  </si>
+  <si>
+    <t>normal normal in pymc3  (esercizio su predictive;  spiegato fino a student likelihood, inclusa)</t>
+  </si>
+  <si>
+    <t>finire normal normal model; presentazione progetto; intro hyp test</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -255,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
@@ -277,7 +280,11 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -621,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D01C0E-36DF-B748-B91C-92F7CA25FEEF}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="184" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="184" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -979,7 +986,7 @@
         <v>44858</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D33" s="9"/>
     </row>
@@ -991,8 +998,8 @@
         <f>B33+3</f>
         <v>44861</v>
       </c>
-      <c r="C34" s="11" t="s">
-        <v>43</v>
+      <c r="C34" t="s">
+        <v>42</v>
       </c>
       <c r="D34" s="9"/>
     </row>
@@ -1000,25 +1007,25 @@
       <c r="A35" s="13">
         <v>7</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="14">
         <f>B33+7</f>
         <v>44865</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>41</v>
+      <c r="C35" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="D35" s="9"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="A36" s="13">
         <v>7</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="8">
         <f>B35+3</f>
         <v>44868</v>
       </c>
-      <c r="C36" s="11" t="s">
-        <v>44</v>
+      <c r="C36" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="D36" s="9"/>
     </row>
@@ -1030,8 +1037,8 @@
         <f>B35+7</f>
         <v>44872</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>45</v>
+      <c r="C37" t="s">
+        <v>44</v>
       </c>
       <c r="D37" s="9"/>
     </row>
@@ -1043,7 +1050,9 @@
         <f>B37+3</f>
         <v>44875</v>
       </c>
-      <c r="C38" s="12"/>
+      <c r="C38" s="12" t="s">
+        <v>2</v>
+      </c>
       <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
minor fix to linear reg
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/BDA-syllabus.xlsx
+++ b/syllabus-and-improv/BDA-syllabus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BD5335-9B90-FD40-8E42-9D2E36C8BDFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DB8411-9A33-2F49-B83E-463D1512D4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -209,16 +209,16 @@
     <t xml:space="preserve">hierarchical  spotify </t>
   </si>
   <si>
-    <t>hierarhical spotify (exericises); lin reg</t>
-  </si>
-  <si>
     <t>revisione progetti</t>
   </si>
   <si>
-    <t>lin reg gerarchica o (AB test??)</t>
-  </si>
-  <si>
-    <t>lin reg gerarchica (o AB test??)</t>
+    <t>hierarhical spotify (exericises); lin reg (fino prior non-informative)</t>
+  </si>
+  <si>
+    <t>lin reg (da prior non-informative in poi)</t>
+  </si>
+  <si>
+    <t>lin reg gerarchica</t>
   </si>
 </sst>
 </file>
@@ -1409,7 +1409,7 @@
         <v>44900</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E45" s="9"/>
     </row>
@@ -1443,7 +1443,7 @@
         <v>44907</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="E47" s="9"/>
     </row>
@@ -1460,7 +1460,7 @@
         <v>44910</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E48" s="9"/>
     </row>
@@ -1491,7 +1491,7 @@
         <v>44917</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update notebooks 2 and 3 to be compliant with pymc
</commit_message>
<xml_diff>
--- a/syllabus-and-improv/BDA-syllabus.xlsx
+++ b/syllabus-and-improv/BDA-syllabus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgio/switchdrive/teaching/BayesianProg/bda/syllabus-and-improv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679C31E8-F376-DE47-B1A6-FB7B4A3DBC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF523702-3E4F-1045-92FB-86CC13F7D569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Previsione</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t xml:space="preserve"> lin reg gerarchica ( case study varying slope) + chiedere come organizzare settimana prossima</t>
+  </si>
+  <si>
+    <t>anticipare qui la presentazione progetto??</t>
   </si>
 </sst>
 </file>
@@ -272,12 +275,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -301,8 +298,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,18 +327,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF8CBAD"/>
-        <bgColor rgb="FFE7E6E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -342,12 +339,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -364,37 +377,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="4" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Excel Built-in Good" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -800,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B38" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1016,7 +1022,7 @@
       <c r="B22" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="13" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="7" t="s">
@@ -1034,7 +1040,7 @@
         <f t="shared" ref="B23:B50" si="0">TEXT(WEEKDAY(C23),"dddddd")</f>
         <v>Monday</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="13">
         <v>44823</v>
       </c>
       <c r="D23" s="8" t="s">
@@ -1050,7 +1056,7 @@
         <f t="shared" si="0"/>
         <v>Thursday</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24" s="13">
         <f>C23+3</f>
         <v>44826</v>
       </c>
@@ -1067,7 +1073,7 @@
         <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="13">
         <f>C23+7</f>
         <v>44830</v>
       </c>
@@ -1084,11 +1090,11 @@
         <f t="shared" si="0"/>
         <v>Thursday</v>
       </c>
-      <c r="C26" s="17">
+      <c r="C26" s="18">
         <f>C25+3</f>
         <v>44833</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="17" t="s">
         <v>36</v>
       </c>
       <c r="E26" s="9"/>
@@ -1101,14 +1107,16 @@
         <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="13">
         <f>C25+7</f>
         <v>44837</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="9"/>
+      <c r="E27" s="9" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -1118,7 +1126,7 @@
         <f t="shared" si="0"/>
         <v>Thursday</v>
       </c>
-      <c r="C28" s="16">
+      <c r="C28" s="13">
         <f>C27+3</f>
         <v>44840</v>
       </c>
@@ -1135,7 +1143,7 @@
         <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="13">
         <f>C27+7</f>
         <v>44844</v>
       </c>
@@ -1152,11 +1160,11 @@
         <f t="shared" si="0"/>
         <v>Thursday</v>
       </c>
-      <c r="C30" s="17">
+      <c r="C30" s="18">
         <f>C29+3</f>
         <v>44847</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="17" t="s">
         <v>40</v>
       </c>
       <c r="E30" s="9"/>
@@ -1169,7 +1177,7 @@
         <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
-      <c r="C31" s="16">
+      <c r="C31" s="13">
         <f>C29+7</f>
         <v>44851</v>
       </c>
@@ -1186,7 +1194,7 @@
         <f t="shared" si="0"/>
         <v>Thursday</v>
       </c>
-      <c r="C32" s="16">
+      <c r="C32" s="13">
         <f>C31+3</f>
         <v>44854</v>
       </c>
@@ -1203,7 +1211,7 @@
         <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C33" s="13">
         <f>C31+7</f>
         <v>44858</v>
       </c>
@@ -1220,7 +1228,7 @@
         <f t="shared" si="0"/>
         <v>Thursday</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="13">
         <f>C33+3</f>
         <v>44861</v>
       </c>
@@ -1237,7 +1245,7 @@
         <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
-      <c r="C35" s="16">
+      <c r="C35" s="13">
         <f>C33+7</f>
         <v>44865</v>
       </c>
@@ -1254,11 +1262,11 @@
         <f t="shared" si="0"/>
         <v>Thursday</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C36" s="18">
         <f>C35+3</f>
         <v>44868</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="17" t="s">
         <v>45</v>
       </c>
       <c r="E36" s="9"/>
@@ -1271,7 +1279,7 @@
         <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
-      <c r="C37" s="16">
+      <c r="C37" s="13">
         <f>C35+7</f>
         <v>44872</v>
       </c>
@@ -1288,11 +1296,11 @@
         <f t="shared" si="0"/>
         <v>Thursday</v>
       </c>
-      <c r="C38" s="17">
+      <c r="C38" s="18">
         <f>C37+3</f>
         <v>44875</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="17" t="s">
         <v>46</v>
       </c>
       <c r="E38" s="9"/>
@@ -1305,7 +1313,7 @@
         <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
-      <c r="C39" s="16">
+      <c r="C39" s="13">
         <f>C37+7</f>
         <v>44879</v>
       </c>
@@ -1322,11 +1330,11 @@
         <f t="shared" si="0"/>
         <v>Thursday</v>
       </c>
-      <c r="C40" s="16">
+      <c r="C40" s="13">
         <f>C39+3</f>
         <v>44882</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="10" t="s">
         <v>50</v>
       </c>
       <c r="E40" s="9"/>
@@ -1339,11 +1347,11 @@
         <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
-      <c r="C41" s="20">
+      <c r="C41" s="15">
         <f>C39+7</f>
         <v>44886</v>
       </c>
-      <c r="D41" s="21" t="s">
+      <c r="D41" s="16" t="s">
         <v>53</v>
       </c>
       <c r="E41" s="9"/>
@@ -1356,11 +1364,11 @@
         <f t="shared" si="0"/>
         <v>Thursday</v>
       </c>
-      <c r="C42" s="22">
+      <c r="C42" s="18">
         <f>C41+3</f>
         <v>44889</v>
       </c>
-      <c r="D42" s="23" t="s">
+      <c r="D42" s="17" t="s">
         <v>54</v>
       </c>
       <c r="E42" s="9"/>
@@ -1373,11 +1381,11 @@
         <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
-      <c r="C43" s="16">
+      <c r="C43" s="13">
         <f>C41+7</f>
         <v>44893</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" t="s">
         <v>55</v>
       </c>
       <c r="E43" s="9"/>
@@ -1394,7 +1402,7 @@
         <f>C43+3</f>
         <v>44896</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="19" t="s">
         <v>51</v>
       </c>
       <c r="E44" s="9"/>
@@ -1407,11 +1415,11 @@
         <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
-      <c r="C45" s="16">
+      <c r="C45" s="13">
         <f>C43+7</f>
         <v>44900</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" t="s">
         <v>57</v>
       </c>
       <c r="E45" s="9"/>
@@ -1420,15 +1428,15 @@
       <c r="A46">
         <v>12</v>
       </c>
-      <c r="B46" s="14" t="str">
+      <c r="B46" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Thursday</v>
       </c>
-      <c r="C46" s="19">
+      <c r="C46" s="14">
         <f>C44+7</f>
         <v>44903</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="12" t="s">
         <v>60</v>
       </c>
       <c r="E46" s="9"/>
@@ -1441,11 +1449,11 @@
         <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
-      <c r="C47" s="16">
+      <c r="C47" s="13">
         <f>C45+7</f>
         <v>44907</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="D47" t="s">
         <v>59</v>
       </c>
       <c r="E47" s="9"/>
@@ -1458,11 +1466,11 @@
         <f t="shared" si="0"/>
         <v>Thursday</v>
       </c>
-      <c r="C48" s="16">
+      <c r="C48" s="13">
         <f>C47+3</f>
         <v>44910</v>
       </c>
-      <c r="D48" s="11" t="s">
+      <c r="D48" t="s">
         <v>61</v>
       </c>
       <c r="E48" s="9"/>
@@ -1475,11 +1483,11 @@
         <f t="shared" si="0"/>
         <v>Monday</v>
       </c>
-      <c r="C49" s="16">
+      <c r="C49" s="13">
         <f>C47+7</f>
         <v>44914</v>
       </c>
-      <c r="D49" s="11" t="s">
+      <c r="D49" t="s">
         <v>58</v>
       </c>
       <c r="E49" s="9"/>
@@ -1489,17 +1497,20 @@
         <f t="shared" si="0"/>
         <v>Thursday</v>
       </c>
-      <c r="C50" s="16">
+      <c r="C50" s="13">
         <f>C49+3</f>
         <v>44917</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="D50" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <ignoredErrors>
+    <ignoredError sqref="C48 C44 C42" formula="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>